<commit_message>
docs: se actualizan normas formales y se actualiza project
</commit_message>
<xml_diff>
--- a/02-Diseño/03-Modelo_Relacional/Normas_formales.xlsx
+++ b/02-Diseño/03-Modelo_Relacional/Normas_formales.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
   <si>
     <t>Entidad</t>
   </si>
@@ -92,9 +92,6 @@
     <t>tipo_doc</t>
   </si>
   <si>
-    <t>empresa_proveedora</t>
-  </si>
-  <si>
     <t>categoria</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Noramalizacion SICLOUD</t>
+  </si>
+  <si>
+    <t>empresa_provedor</t>
   </si>
 </sst>
 </file>
@@ -178,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -306,26 +306,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,9 +337,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -368,9 +350,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -388,7 +367,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -651,14 +630,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="10" t="s">
-        <v>25</v>
+      <c r="D2" s="20" t="s">
+        <v>24</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -707,22 +686,22 @@
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="5"/>
@@ -746,7 +725,7 @@
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -759,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="15"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -781,7 +760,7 @@
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -794,7 +773,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="16"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -816,7 +795,7 @@
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -829,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="5"/>
@@ -853,7 +832,7 @@
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -866,7 +845,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J8" s="5"/>
@@ -890,7 +869,7 @@
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -903,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="14"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -925,7 +904,7 @@
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -938,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -960,7 +939,7 @@
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -973,7 +952,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="15"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -995,7 +974,7 @@
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="8" t="s">
@@ -1008,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1030,7 +1009,7 @@
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="8" t="s">
@@ -1043,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="15"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -1065,7 +1044,7 @@
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="8" t="s">
@@ -1078,7 +1057,7 @@
         <v>7</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1100,7 +1079,7 @@
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -1113,7 +1092,7 @@
         <v>7</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="15"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1135,7 +1114,7 @@
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1148,7 +1127,7 @@
         <v>7</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="15"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -1170,7 +1149,7 @@
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="8" t="s">
@@ -1183,7 +1162,7 @@
         <v>7</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1205,7 +1184,7 @@
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -1218,7 +1197,7 @@
         <v>7</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="14"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1240,7 +1219,7 @@
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="8" t="s">
@@ -1255,7 +1234,9 @@
       <c r="H19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="16"/>
+      <c r="I19" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1277,8 +1258,8 @@
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="14" t="s">
-        <v>22</v>
+      <c r="D20" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>7</v>
@@ -1289,8 +1270,10 @@
       <c r="G20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="15"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1312,8 +1295,8 @@
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="14" t="s">
-        <v>23</v>
+      <c r="D21" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>7</v>
@@ -1325,7 +1308,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J21" s="5"/>
@@ -1349,22 +1332,20 @@
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="19" t="s">
-        <v>24</v>
+      <c r="D22" s="17" t="s">
+        <v>23</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22" t="s">
-        <v>7</v>
-      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>

</xml_diff>

<commit_message>
docs: Se agrega la normalizaciòn de la base de datos.
</commit_message>
<xml_diff>
--- a/02-Diseño/03-Modelo_Relacional/Normas_formales.xlsx
+++ b/02-Diseño/03-Modelo_Relacional/Normas_formales.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="29">
   <si>
     <t>Entidad</t>
   </si>
@@ -103,6 +103,15 @@
   <si>
     <t>empresa_provedor</t>
   </si>
+  <si>
+    <t>tipo_pago</t>
+  </si>
+  <si>
+    <t>log_error</t>
+  </si>
+  <si>
+    <t>servidor_correo</t>
+  </si>
 </sst>
 </file>
 
@@ -178,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -286,6 +295,32 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -301,6 +336,118 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -310,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,16 +505,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -630,14 +816,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1328,24 +1514,24 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1363,16 +1549,24 @@
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="D23" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="30"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -1390,16 +1584,24 @@
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="D24" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="32"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -1417,16 +1619,24 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="D25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="20"/>
+      <c r="I25" s="33"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>

</xml_diff>